<commit_message>
Updated schema, excel files, database (data) population script
</commit_message>
<xml_diff>
--- a/MySQL/guests_db.xlsx
+++ b/MySQL/guests_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant\Desktop\mThreeInClass\MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DCA4DD-D4A7-4F6E-9A18-A09BC242B2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE07BA4F-5012-4654-9773-2907344A1415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{8A2080AE-6A9F-4371-AD15-F66107BAA796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A2080AE-6A9F-4371-AD15-F66107BAA796}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>IA</t>
   </si>
   <si>
-    <t>(291) 553-0508</t>
-  </si>
-  <si>
     <t>Bettyann Seery</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>AK</t>
   </si>
   <si>
-    <t>(478) 277-9632</t>
-  </si>
-  <si>
     <t>Duane Cullison</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t>TX</t>
   </si>
   <si>
-    <t>(308) 494-0198</t>
-  </si>
-  <si>
     <t>Karie Yang</t>
   </si>
   <si>
@@ -94,9 +85,6 @@
     <t>NJ</t>
   </si>
   <si>
-    <t>(214) 730-0298</t>
-  </si>
-  <si>
     <t>Aurore Lipton</t>
   </si>
   <si>
@@ -109,9 +97,6 @@
     <t>MI</t>
   </si>
   <si>
-    <t>(377) 507-0974</t>
-  </si>
-  <si>
     <t>Zachery Luechtefeld</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t>CO</t>
   </si>
   <si>
-    <t>(814) 485-2615</t>
-  </si>
-  <si>
     <t>Jeremiah Pendergrass</t>
   </si>
   <si>
@@ -139,9 +121,6 @@
     <t>IL</t>
   </si>
   <si>
-    <t>(279) 491-0960</t>
-  </si>
-  <si>
     <t>Walter Holaway</t>
   </si>
   <si>
@@ -154,9 +133,6 @@
     <t>RI</t>
   </si>
   <si>
-    <t>(446) 396-6785</t>
-  </si>
-  <si>
     <t>Wilfred Vise</t>
   </si>
   <si>
@@ -169,9 +145,6 @@
     <t>NY</t>
   </si>
   <si>
-    <t>(834) 727-1001</t>
-  </si>
-  <si>
     <t>Maritza Tilton</t>
   </si>
   <si>
@@ -184,9 +157,6 @@
     <t>VA</t>
   </si>
   <si>
-    <t>(446) 351-6860</t>
-  </si>
-  <si>
     <t>Joleen Tison</t>
   </si>
   <si>
@@ -199,7 +169,37 @@
     <t>PA</t>
   </si>
   <si>
-    <t>(231) 893-2755</t>
+    <t>291 553-0508</t>
+  </si>
+  <si>
+    <t>478 277-9632</t>
+  </si>
+  <si>
+    <t>308 494-0198</t>
+  </si>
+  <si>
+    <t>214 730-0298</t>
+  </si>
+  <si>
+    <t>377 507-0974</t>
+  </si>
+  <si>
+    <t>814 485-2615</t>
+  </si>
+  <si>
+    <t>279 491-0960</t>
+  </si>
+  <si>
+    <t>446 396-6785</t>
+  </si>
+  <si>
+    <t>834 727-1001</t>
+  </si>
+  <si>
+    <t>446 351-6860</t>
+  </si>
+  <si>
+    <t>231 893-2755</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,201 +590,201 @@
         <v>51501</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>99654</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>78552</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="1">
         <v>8096</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>48601</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1">
         <v>80003</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1">
         <v>60099</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1">
         <v>2864</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1">
         <v>13126</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1">
         <v>22015</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1">
         <v>19026</v>

</xml_diff>